<commit_message>
Integrated Login and Passed all Assignment cases
</commit_message>
<xml_diff>
--- a/database/User_Passwords.xlsx
+++ b/database/User_Passwords.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/advait/Desktop/gitpositories/sc2002/database/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0147D4EA-C5C9-584C-9DFB-9F727081316C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2128B64E-A2AF-794F-AF7B-4A6D3BC6980D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3620" yWindow="2680" windowWidth="23260" windowHeight="12580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,19 +36,280 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="89">
   <si>
     <t>UserID</t>
   </si>
   <si>
     <t>Password</t>
+  </si>
+  <si>
+    <t>YCHERN@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>KOH1@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>BR015@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>CT113@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>YCN019@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>DL007@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>DON84@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>ELI34@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>LE51@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>SL22@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>AKY013@e.ntu.edu.sg;</t>
+  </si>
+  <si>
+    <t>ASMADHUKUMAR@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASSOURIN@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ANUPAM@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ANWITAMAN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ARVINDE@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>BOAN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASWTCAI@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASTJCHAM@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASSCHAN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>CCLOY@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASLTCHIA@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASESCHNG@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>GAOCONG@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASDRAJAN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASDOUGLAS@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>DNIYATO@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>CAMBRIA@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>xyfan@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASWBGOH@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>CTGUAN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>YHE@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASSYHUANG@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASSCHUI@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>SRJOTY@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>YPKE@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ADAMSKONG@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASCKKWOH@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASSKLAM@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASCTLAU@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>EBSLEE@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>boyang.li@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASFLI@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>LIMO@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>YI_LI@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>gslin@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>SHANG-WEI.LIN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>WSLIN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>LIU@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>YANGLIU@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ziwei.liu@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>anhtuan.luu@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>YRLOKE@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>C.LONG@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>SHIJIAN.LU@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>JUNLUO@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>siqiang.luo@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>MSABRY@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>AWKNG@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>HLOH@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASYSOng@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>OFERNANDO@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>SINNOPAN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>MKMQIAN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASHCQUEK@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASJAGATH@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASHSSEAH@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ZQSHEN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>SMITHA@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASSOURAV@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>AXSUN@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>cheewei.tan@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>TANRUI@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASXYTANG@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>kianboon.tay@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASTSRIKAN@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>vidya.sudarshan@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASCHVUN@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>YGWEN@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>ASCKYEO@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>HAN.YU@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>HANWANGZHANG@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ZHANGJ@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>tianwei.zhang@ntu.edu.sg</t>
+  </si>
+  <si>
+    <t>JUNZHAO@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>ASJMZHENG@NTU.EDU.SG</t>
+  </si>
+  <si>
+    <t>password</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -78,6 +339,19 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Microsoft Sans Serif"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -100,10 +374,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -385,65 +662,733 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.5" customWidth="1"/>
+    <col min="1" max="1" width="30.5" style="4" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="2"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
+      <c r="A2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="1"/>
+      <c r="A3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="1"/>
+      <c r="A4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B5" s="1"/>
+      <c r="A5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B6" s="1"/>
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B7" s="1"/>
+      <c r="A7" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B8" s="1"/>
+      <c r="A8" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
+      <c r="A9" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B10" s="1"/>
+      <c r="A10" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B11" s="1"/>
+      <c r="A11" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="B12" s="1"/>
+      <c r="A12" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B16" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A17" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B17" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B18" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A19" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A20" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B20" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B21" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A22" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B22" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B23" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B24" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A25" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A26" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B26" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A27" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B27" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A28" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B28" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A29" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B29" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A30" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A31" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B31" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A32" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B32" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A33" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B33" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B35" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B36" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B37" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B38" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B39" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A40" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B40" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A41" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A42" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B42" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A44" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A45" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B45" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A46" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B46" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A47" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B47" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A48" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B48" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A49" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A51" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B51" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A52" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A53" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A54" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A55" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B55" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A56" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B56" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A57" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="B57" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A58" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="B58" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="B59" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A60" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B60" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A61" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B61" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A62" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B62" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B63" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A64" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B64" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A65" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="B65" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A66" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B66" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A67" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B67" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A68" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B68" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A69" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B69" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A70" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B70" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A71" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B71" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A72" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B72" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B73" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A74" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B74" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B75" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A76" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B76" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A77" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B77" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A78" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B78" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A79" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B79" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A80" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="B80" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A81" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B81" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A82" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B82" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A83" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B83" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A84" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B84" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A85" s="4" t="s">
+        <v>85</v>
+      </c>
+      <c r="B85" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A86" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B86" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A87" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B87" t="s">
+        <v>88</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" xr:uid="{8FBD9A16-151B-264A-95B8-B38F36D91950}"/>
+    <hyperlink ref="A3" r:id="rId2" xr:uid="{A2F8D1BD-577F-104B-B766-23083560D48F}"/>
+    <hyperlink ref="A4" r:id="rId3" xr:uid="{111A1BCC-A589-3340-A2ED-8B2C301B03B9}"/>
+    <hyperlink ref="A5" r:id="rId4" xr:uid="{20983774-8045-014C-BE6A-8726E7614643}"/>
+    <hyperlink ref="A6" r:id="rId5" xr:uid="{7C062B76-2B90-4345-BE92-C162A088A32A}"/>
+    <hyperlink ref="A7" r:id="rId6" xr:uid="{F9F30DFC-D10B-654E-95D3-23DD6489E17A}"/>
+    <hyperlink ref="A8" r:id="rId7" xr:uid="{79034A79-BA40-1044-94F6-016850DF84ED}"/>
+    <hyperlink ref="A9" r:id="rId8" xr:uid="{C0D17BAC-1C60-5649-9D00-003183979034}"/>
+    <hyperlink ref="A10" r:id="rId9" xr:uid="{48E31C89-CAF9-C94B-9F37-2B96619B8CF2}"/>
+    <hyperlink ref="A11" r:id="rId10" xr:uid="{66F3E6E7-D805-7643-9EBC-6F627949A01B}"/>
+    <hyperlink ref="A12" r:id="rId11" xr:uid="{E63B3A2D-D37D-9245-930C-630DF01BA444}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId12"/>
 </worksheet>
 </file>
</xml_diff>